<commit_message>
birth and firm services
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/testscript_data/testscript1.xlsx
+++ b/Demo/src/test/resources/testscript_data/testscript1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshitha\Downloads\Demo\Demo\src\test\resources\testscript_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Meeseva_Automation\Demo\src\test\resources\testscript_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BC7D1F-2BB0-4EFE-B265-59745CF48CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F612A7C-A4F4-4FF2-B6EE-B32993614A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{BB50BD55-AD61-476C-AEBF-91414C792521}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="7" xr2:uid="{BB50BD55-AD61-476C-AEBF-91414C792521}"/>
   </bookViews>
   <sheets>
     <sheet name="MEE_INCOME_SERVICE" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="OBC_USER_DATA" sheetId="6" r:id="rId4"/>
     <sheet name="MEE_RESIDENCE_SERVICE" sheetId="7" r:id="rId5"/>
     <sheet name="Residence_User_Data" sheetId="8" r:id="rId6"/>
+    <sheet name="BIRTH_GHMC" sheetId="9" r:id="rId7"/>
+    <sheet name="GHMC_Birth_Data" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -101,8 +103,32 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Vijay</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{44472F0C-6300-4770-9A26-D6FF628EBDFB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Updated on 4/11/2024</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="131">
   <si>
     <t>Harshitha</t>
   </si>
@@ -451,6 +477,56 @@
   </si>
   <si>
     <t>04/12/2001</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>This testcase validates user can able to apply for Birth certificate GHMC by entering all valid details.</t>
+  </si>
+  <si>
+    <t>1.User should be able to apply for the certificate
+2.System will display the Receipt of applied successfully by the user as confirmation.
+3. user can able to print the birth certificate instantly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEE_Birth_Certificate_FT_01 : Validates the Birth and Death Certificate GHMC Application Service </t>
+  </si>
+  <si>
+    <t>GHMC_BIRTH_CERTIFICATE_SERVICE</t>
+  </si>
+  <si>
+    <t>Informant Name</t>
+  </si>
+  <si>
+    <t>Informant Address</t>
+  </si>
+  <si>
+    <t>Purpose of Certificate</t>
+  </si>
+  <si>
+    <t>No of Copies</t>
+  </si>
+  <si>
+    <t>1/2h Address</t>
+  </si>
+  <si>
+    <t>543212</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>55h test</t>
+  </si>
+  <si>
+    <t>567898</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -754,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -799,6 +875,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -850,10 +930,12 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,6 +1107,61 @@
         <a:xfrm>
           <a:off x="402374" y="0"/>
           <a:ext cx="2140801" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>402374</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2543175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>542925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC724DBC-2195-4246-AA04-1F6D49176C38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="402374" y="0"/>
+          <a:ext cx="2140801" cy="1038225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1339,60 +1476,60 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="47.1796875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.81640625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="26"/>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="27"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="28"/>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1409,7 +1546,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
@@ -1426,7 +1563,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
@@ -1465,25 +1602,25 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.26953125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
@@ -1497,7 +1634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -1511,7 +1648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
@@ -1525,7 +1662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>49</v>
       </c>
@@ -1539,7 +1676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>50</v>
       </c>
@@ -1553,7 +1690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>51</v>
       </c>
@@ -1567,7 +1704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>52</v>
       </c>
@@ -1581,7 +1718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>53</v>
       </c>
@@ -1595,7 +1732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>54</v>
       </c>
@@ -1609,7 +1746,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>55</v>
       </c>
@@ -1640,61 +1777,61 @@
       <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="51.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.26953125" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" customWidth="1"/>
     <col min="5" max="5" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="26"/>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="27"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="28"/>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1711,7 +1848,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>64</v>
       </c>
@@ -1724,7 +1861,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>66</v>
       </c>
@@ -1737,14 +1874,14 @@
       <c r="D8" s="5"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1773,25 +1910,25 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>46</v>
       </c>
@@ -1805,7 +1942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>68</v>
       </c>
@@ -1819,7 +1956,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>72</v>
       </c>
@@ -1833,7 +1970,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>51</v>
       </c>
@@ -1847,7 +1984,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>52</v>
       </c>
@@ -1861,7 +1998,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>53</v>
       </c>
@@ -1875,7 +2012,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>54</v>
       </c>
@@ -1889,7 +2026,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>84</v>
       </c>
@@ -1916,64 +2053,64 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+      <selection activeCell="E7" sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="44.81640625" customWidth="1"/>
+    <col min="2" max="2" width="34.7265625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="24"/>
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="26"/>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="27"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="28"/>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1990,7 +2127,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>86</v>
       </c>
@@ -2000,10 +2137,12 @@
       <c r="C7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>89</v>
       </c>
@@ -2034,29 +2173,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6163837-592A-487C-920D-4346FEDEC5EA}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.7265625" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>92</v>
       </c>
@@ -2070,7 +2209,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>68</v>
       </c>
@@ -2084,7 +2223,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>93</v>
       </c>
@@ -2098,7 +2237,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>51</v>
       </c>
@@ -2112,7 +2251,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
@@ -2126,7 +2265,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>53</v>
       </c>
@@ -2140,7 +2279,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>54</v>
       </c>
@@ -2154,7 +2293,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>95</v>
       </c>
@@ -2168,11 +2307,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="19" t="s">
         <v>112</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -2189,4 +2328,219 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9113F76-C769-477C-9435-AD1D2FFE4750}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="42.36328125" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="3" max="3" width="38.08984375" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" customWidth="1"/>
+    <col min="5" max="5" width="25.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="26"/>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="27"/>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="1:5" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="28"/>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDF441F-B1A5-434D-9DE9-9F5719B02E22}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.6328125" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="38"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
registration of firm is created
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/testscript_data/testscript1.xlsx
+++ b/Demo/src/test/resources/testscript_data/testscript1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Meeseva_Automation\Demo\src\test\resources\testscript_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshitha\Downloads\Demo\Demo\src\test\resources\testscript_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F612A7C-A4F4-4FF2-B6EE-B32993614A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EE20AE-47A5-4FE4-8FE0-774917D32CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="7" xr2:uid="{BB50BD55-AD61-476C-AEBF-91414C792521}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="9" xr2:uid="{BB50BD55-AD61-476C-AEBF-91414C792521}"/>
   </bookViews>
   <sheets>
     <sheet name="MEE_INCOME_SERVICE" sheetId="3" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="Residence_User_Data" sheetId="8" r:id="rId6"/>
     <sheet name="BIRTH_GHMC" sheetId="9" r:id="rId7"/>
     <sheet name="GHMC_Birth_Data" sheetId="10" r:id="rId8"/>
+    <sheet name="MEE_REG_OF_FIRM" sheetId="11" r:id="rId9"/>
+    <sheet name="Firm_User_Data" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -127,8 +129,32 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Vijay</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{07CDE029-E656-49C0-AEEB-997DC6265377}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Updated on 4/11/2024</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="221">
   <si>
     <t>Harshitha</t>
   </si>
@@ -215,12 +241,6 @@
     <t>WAP4158789658</t>
   </si>
   <si>
-    <t>MEE_INCOME_SERVICE_FT_01 : Validate Income Certificate Service</t>
-  </si>
-  <si>
-    <t>MEE_INCOME_SERVICE_FT_DEPT_01 : Validating Income certificate Details at Deaprtment Side</t>
-  </si>
-  <si>
     <t>This testcase validates that user entered details are fetched exactly at the department side</t>
   </si>
   <si>
@@ -325,15 +345,9 @@
     <t>ACTUAL RESULT</t>
   </si>
   <si>
-    <t xml:space="preserve">MEE_OBC_FT_01 : Validates the OBC Application Service </t>
-  </si>
-  <si>
     <t>This testcase validates user can able to apply for OBC certificate by entering all valid details.</t>
   </si>
   <si>
-    <t>MEE_OBC_DEPT_FT_01 : Validating the OBC certificate Application Form details at the Department side</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
@@ -391,16 +405,10 @@
     <t>35000</t>
   </si>
   <si>
-    <t xml:space="preserve">MEE_Residence_FT_01 : Validates the Residence Application Service </t>
-  </si>
-  <si>
     <t>This testcase validates user can able to apply for Residence certificate by entering all valid details.</t>
   </si>
   <si>
     <t>MEE_RESIDENCE_SERVICE</t>
-  </si>
-  <si>
-    <t>MEE_RESIDENCE_DEPT_FT_01 : Validates the Residence certificate Application Form details at the Department side</t>
   </si>
   <si>
     <t>1. data need to be matched as user entered
@@ -490,9 +498,6 @@
 3. user can able to print the birth certificate instantly</t>
   </si>
   <si>
-    <t xml:space="preserve">MEE_Birth_Certificate_FT_01 : Validates the Birth and Death Certificate GHMC Application Service </t>
-  </si>
-  <si>
     <t>GHMC_BIRTH_CERTIFICATE_SERVICE</t>
   </si>
   <si>
@@ -527,6 +532,299 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Test case validates that user can able to apply the firm registration by entering valid details</t>
+  </si>
+  <si>
+    <t>1. user applied successfully to register the firm in IGRS department.
+2. After applied, system will displayed the receipt for successful transaction</t>
+  </si>
+  <si>
+    <t>Test case validates that user details are correctly fetched at the department side</t>
+  </si>
+  <si>
+    <t>MEE_REV_INCOME_SERVICE_FT_001 : Validate Income Certificate Service</t>
+  </si>
+  <si>
+    <t>MEE_REV_INCOME_SERVICE_FT_002 : Validating Income certificate Details at Deaprtment Side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEE_REV_OBC_FT_001 : Validates the OBC Application Service </t>
+  </si>
+  <si>
+    <t>MEE_REV_OBC_FT_002 : Validating the OBC certificate Application Form details at the Department side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEE_REV_RESIDENCE_FT_001 : Validates the Residence Application Service </t>
+  </si>
+  <si>
+    <t>MEE_REV_RESIDENCE_FT_002 : Validates the Residence certificate Application Form details at the Department side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEE_GHMC_Birth_Certificate_FT_001 : Validates the Birth and Death Certificate GHMC Application Service </t>
+  </si>
+  <si>
+    <t>MEE_IGRS_REG_OF_FIRM_FT_001 : Validates the Registration of Firm service in IGRS department</t>
+  </si>
+  <si>
+    <t>MEE_IGRS_REG_OF_FIRM_FT_002 : Validates the user details in the Department level</t>
+  </si>
+  <si>
+    <t>1. DLF - if user details are matched, DLF can forward the application to DR
+2. DR - In DR login, if user details are matched then DR user can take necessary action on the application</t>
+  </si>
+  <si>
+    <t>MEE_REG_OF_FIRM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name </t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Door no</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>Mobile no</t>
+  </si>
+  <si>
+    <t>Firm Name</t>
+  </si>
+  <si>
+    <t>Firm Duration From</t>
+  </si>
+  <si>
+    <t>Firm Duration To</t>
+  </si>
+  <si>
+    <t>Applicant Fields</t>
+  </si>
+  <si>
+    <t>Principal Address</t>
+  </si>
+  <si>
+    <t>Partner Details</t>
+  </si>
+  <si>
+    <t>Partner Name</t>
+  </si>
+  <si>
+    <t>Partner Surname</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Joining Date</t>
+  </si>
+  <si>
+    <t>Document Name</t>
+  </si>
+  <si>
+    <t>Affidavit</t>
+  </si>
+  <si>
+    <t>Form 1 - English Version</t>
+  </si>
+  <si>
+    <t>Partnership deed</t>
+  </si>
+  <si>
+    <t>Self  signed declaration</t>
+  </si>
+  <si>
+    <t>test first</t>
+  </si>
+  <si>
+    <t>testsurname</t>
+  </si>
+  <si>
+    <t>12d</t>
+  </si>
+  <si>
+    <t>test street</t>
+  </si>
+  <si>
+    <t>test village</t>
+  </si>
+  <si>
+    <t>545555</t>
+  </si>
+  <si>
+    <t>ASHOKA VENTURE FIRM</t>
+  </si>
+  <si>
+    <t>12/06/2018</t>
+  </si>
+  <si>
+    <t>23 test</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>village</t>
+  </si>
+  <si>
+    <t>567656</t>
+  </si>
+  <si>
+    <t>surnameA</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>09/09/2020</t>
+  </si>
+  <si>
+    <t>56df</t>
+  </si>
+  <si>
+    <t>streetA</t>
+  </si>
+  <si>
+    <t>villageA</t>
+  </si>
+  <si>
+    <t>564442</t>
+  </si>
+  <si>
+    <t>PartnerB</t>
+  </si>
+  <si>
+    <t>PartnerA</t>
+  </si>
+  <si>
+    <t>surnameB</t>
+  </si>
+  <si>
+    <t>streetB</t>
+  </si>
+  <si>
+    <t>villageB</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>12/02/2022</t>
+  </si>
+  <si>
+    <t>65a test</t>
+  </si>
+  <si>
+    <t>569898</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Partnership</t>
+  </si>
+  <si>
+    <t>Declaration</t>
+  </si>
+  <si>
+    <t>Kishore</t>
+  </si>
+  <si>
+    <t>Doda</t>
+  </si>
+  <si>
+    <t>Degala</t>
+  </si>
+  <si>
+    <t>Madhuri</t>
+  </si>
+  <si>
+    <t>55f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-88f </t>
+  </si>
+  <si>
+    <t>Teacher's colony</t>
+  </si>
+  <si>
+    <t>NTR colony</t>
+  </si>
+  <si>
+    <t>547855</t>
+  </si>
+  <si>
+    <t>547558</t>
+  </si>
+  <si>
+    <t>MADHURI SPORTS ACADEMY</t>
+  </si>
+  <si>
+    <t>LAKSHMI FOODS</t>
+  </si>
+  <si>
+    <t>14/07/2015</t>
+  </si>
+  <si>
+    <t>10/02/2020</t>
+  </si>
+  <si>
+    <t>indefinite</t>
+  </si>
+  <si>
+    <t>45 test</t>
+  </si>
+  <si>
+    <t>Nagole</t>
+  </si>
+  <si>
+    <t>88c</t>
+  </si>
+  <si>
+    <t>lakshmi puram</t>
+  </si>
+  <si>
+    <t>jubilee hills</t>
+  </si>
+  <si>
+    <t>547775</t>
+  </si>
+  <si>
+    <t>547723</t>
+  </si>
+  <si>
+    <t>banjara hills</t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>28/11/2017</t>
+  </si>
+  <si>
+    <t>23b</t>
+  </si>
+  <si>
+    <t>Prakash Nagar</t>
+  </si>
+  <si>
+    <t>547743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service Name </t>
+  </si>
+  <si>
+    <t>Registration of Firm</t>
   </si>
 </sst>
 </file>
@@ -830,7 +1128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -875,10 +1173,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -933,9 +1230,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1162,6 +1471,61 @@
         <a:xfrm>
           <a:off x="402374" y="0"/>
           <a:ext cx="2140801" cy="1038225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3581400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BC9157C-6F33-4627-ADB8-F270F9BE9E16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="533400" y="0"/>
+          <a:ext cx="3048000" cy="904875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1473,63 +1837,63 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.1796875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.81640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="47.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26"/>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="28"/>
+      <c r="C3" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1543,12 +1907,12 @@
         <v>19</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>24</v>
@@ -1556,28 +1920,28 @@
       <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
-        <v>35</v>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>61</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1594,6 +1958,448 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE9E1A2-EDD3-45F3-9AB6-987D09D82C86}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B26:D26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EF98D6-20F0-45CC-BFE8-C955459C2233}">
   <dimension ref="A1:D11"/>
@@ -1602,27 +2408,27 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.26953125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.26953125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -1634,12 +2440,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -1648,12 +2454,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>1</v>
@@ -1662,12 +2468,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>2</v>
@@ -1676,9 +2482,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>27</v>
@@ -1690,12 +2496,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>3</v>
@@ -1704,12 +2510,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -1718,12 +2524,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>5</v>
@@ -1732,32 +2538,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1774,64 +2580,64 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.7265625" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" customWidth="1"/>
-    <col min="3" max="3" width="28.453125" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" customWidth="1"/>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26"/>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="1:5" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="28"/>
+      <c r="C3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="C4" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1845,15 +2651,15 @@
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>25</v>
@@ -1861,32 +2667,32 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="11"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1910,27 +2716,27 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -1942,102 +2748,102 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="D7" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="C8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="B9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2053,64 +2859,64 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="A1:E7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.81640625" customWidth="1"/>
-    <col min="2" max="2" width="34.7265625" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26"/>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="28"/>
+      <c r="C3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="C4" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -2124,35 +2930,37 @@
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
-        <v>115</v>
+      <c r="D7" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="E8" s="11"/>
     </row>
   </sheetData>
@@ -2177,27 +2985,27 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7265625" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -2209,116 +3017,116 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="C7" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="D7" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="5" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="D9" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2335,63 +3143,63 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.36328125" customWidth="1"/>
-    <col min="2" max="2" width="31.26953125" customWidth="1"/>
-    <col min="3" max="3" width="38.08984375" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" customWidth="1"/>
-    <col min="5" max="5" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26"/>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="1:5" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="28"/>
+      <c r="C3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="42.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="C4" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -2405,18 +3213,18 @@
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="91" customHeight="1" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="90.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="11"/>
@@ -2439,62 +3247,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDF441F-B1A5-434D-9DE9-9F5719B02E22}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6328125" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="38"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>22</v>
@@ -2503,37 +3311,37 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2543,4 +3351,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3934AC55-9144-4095-9900-EB6990E3B202}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
dlf dept is created
</commit_message>
<xml_diff>
--- a/Demo/src/test/resources/testscript_data/testscript1.xlsx
+++ b/Demo/src/test/resources/testscript_data/testscript1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harshitha\Downloads\Demo\Demo\src\test\resources\testscript_data\"/>
     </mc:Choice>
@@ -26,7 +26,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="221">
   <si>
     <t>Harshitha</t>
   </si>
@@ -831,6 +831,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1842,11 +1843,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="46.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="47.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="46.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
@@ -1968,10 +1969,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="40.42578125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="26.7109375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="20.7109375" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2410,10 +2411,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2585,11 +2586,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="51.7109375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="33.28515625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="28.42578125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="23.7109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="50.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
@@ -2718,10 +2719,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="21.140625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="19.28515625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="19.85546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2864,11 +2865,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="44.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="43.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="26.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
@@ -2987,10 +2988,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="40.7109375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="16.5703125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="14.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3148,11 +3149,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="42.42578125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="31.28515625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="38.140625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="25.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
@@ -3253,9 +3254,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="27.5703125" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="16.28515625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="14.42578125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3363,11 +3364,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="56.28515625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="31.42578125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="42.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="25.5703125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="36.85546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
@@ -3442,7 +3443,9 @@
       <c r="C7" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" t="s">
+        <v>109</v>
+      </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">

</xml_diff>